<commit_message>
fixed model, views, serializers code creation
</commit_message>
<xml_diff>
--- a/CRUDCreateCode/data/input/models/CRM.xlsx
+++ b/CRUDCreateCode/data/input/models/CRM.xlsx
@@ -8,24 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkax/dev/aimonetize/Backend/DjangoBasic/CRUDCreateCode/data/input/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701CDFD9-20D1-6644-955E-3D9DD3A80E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6774455-D790-4D40-A01C-A9C4018EC5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="760" windowWidth="26180" windowHeight="18880" activeTab="1" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
+    <workbookView xWindow="4060" yWindow="760" windowWidth="26180" windowHeight="18880" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="model" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId2"/>
-    <sheet name="model_functions" sheetId="7" r:id="rId3"/>
-    <sheet name="help" sheetId="11" r:id="rId4"/>
-    <sheet name="imports" sheetId="12" r:id="rId5"/>
-    <sheet name="signals" sheetId="10" r:id="rId6"/>
-    <sheet name="serializers" sheetId="2" r:id="rId7"/>
-    <sheet name="views" sheetId="3" r:id="rId8"/>
-    <sheet name="urls" sheetId="4" r:id="rId9"/>
-    <sheet name="forms" sheetId="6" r:id="rId10"/>
-    <sheet name="html" sheetId="5" r:id="rId11"/>
-    <sheet name="apps" sheetId="13" r:id="rId12"/>
-    <sheet name="admin" sheetId="14" r:id="rId13"/>
+    <sheet name="model" sheetId="15" r:id="rId1"/>
+    <sheet name="model_functions" sheetId="7" r:id="rId2"/>
+    <sheet name="help" sheetId="11" r:id="rId3"/>
+    <sheet name="imports" sheetId="12" r:id="rId4"/>
+    <sheet name="signals" sheetId="10" r:id="rId5"/>
+    <sheet name="serializers" sheetId="2" r:id="rId6"/>
+    <sheet name="views" sheetId="3" r:id="rId7"/>
+    <sheet name="urls" sheetId="4" r:id="rId8"/>
+    <sheet name="forms" sheetId="6" r:id="rId9"/>
+    <sheet name="html" sheetId="5" r:id="rId10"/>
+    <sheet name="apps" sheetId="13" r:id="rId11"/>
+    <sheet name="admin" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="124">
   <si>
     <t>Variable</t>
   </si>
@@ -78,24 +77,6 @@
   </si>
   <si>
     <t>ForeignKey</t>
-  </si>
-  <si>
-    <t>basic</t>
-  </si>
-  <si>
-    <t>"html"</t>
-  </si>
-  <si>
-    <t>create</t>
-  </si>
-  <si>
-    <t>delete</t>
-  </si>
-  <si>
-    <t>retrieve</t>
-  </si>
-  <si>
-    <t>update</t>
   </si>
   <si>
     <t>functions</t>
@@ -429,22 +410,40 @@
   </si>
   <si>
     <t>"History"</t>
+  </si>
+  <si>
+    <t>created_at</t>
+  </si>
+  <si>
+    <t>models.DateTimeField(auto_now_add=True)</t>
+  </si>
+  <si>
+    <t>"created_at"</t>
+  </si>
+  <si>
+    <t>updated_at</t>
+  </si>
+  <si>
+    <t>models.DateTimeField(auto_now=True)</t>
+  </si>
+  <si>
+    <t>"updated_at"</t>
+  </si>
+  <si>
+    <t>app_name</t>
+  </si>
+  <si>
+    <t>CRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -796,499 +795,1279 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E15A4BF7-DFDE-D24F-85FE-657339D228CC}">
-  <dimension ref="A1:Y66"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FEED97D-C3FC-F94F-8D67-5465F059E3CB}">
+  <dimension ref="A1:Z72"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="32.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" customWidth="1"/>
-    <col min="7" max="12" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="26.6640625" customWidth="1"/>
+    <col min="6" max="6" width="32.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="13" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
       <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="U1" t="s">
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="V2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="V1" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
+      </c>
+      <c r="R3" s="2"/>
+      <c r="V3" s="2">
+        <v>1</v>
+      </c>
+      <c r="X3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="V4" s="2">
+        <v>1</v>
+      </c>
+      <c r="X4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>94</v>
+      </c>
+      <c r="V5" s="2">
+        <v>1</v>
+      </c>
+      <c r="X5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="2">
+        <v>1</v>
+      </c>
+      <c r="X6" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" t="s">
+        <v>118</v>
+      </c>
+      <c r="X8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" t="s">
+        <v>121</v>
+      </c>
+      <c r="X9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>97</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="X10" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="V11" s="2">
+        <v>1</v>
+      </c>
+      <c r="X11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" t="s">
+        <v>98</v>
+      </c>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="V12" s="2">
+        <v>1</v>
+      </c>
+      <c r="X12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" t="s">
+        <v>118</v>
+      </c>
+      <c r="X14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E15" t="s">
+        <v>120</v>
+      </c>
+      <c r="F15" t="s">
+        <v>121</v>
+      </c>
+      <c r="X15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="Y2" s="2"/>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="Y3" s="2"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
         <v>99</v>
       </c>
-      <c r="C4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="Y4" s="2"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" t="s">
-        <v>100</v>
-      </c>
-      <c r="U5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="Y5" s="2"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C6" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" t="s">
-        <v>69</v>
-      </c>
-      <c r="U6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="Y6" s="2"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="S16" s="2"/>
+      <c r="V16" s="2">
+        <v>1</v>
+      </c>
+      <c r="X16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
         <v>118</v>
       </c>
-      <c r="B7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" t="s">
-        <v>103</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="Y8" s="2"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="Y9" s="2"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" t="s">
-        <v>104</v>
-      </c>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="Y10" s="2"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
-      <c r="R12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="W12" s="2"/>
-      <c r="Y12" s="2"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" t="s">
-        <v>119</v>
-      </c>
-      <c r="C13" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" t="s">
-        <v>66</v>
-      </c>
-      <c r="S16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="Y16" s="2"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="X18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
         <v>119</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" t="s">
         <v>120</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="Y20" s="2"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="Y21" s="2"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="U32" s="2"/>
-      <c r="W32" s="2"/>
-      <c r="Y32" s="2"/>
-    </row>
-    <row r="33" spans="15:25" x14ac:dyDescent="0.2">
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="W33" s="2"/>
-      <c r="Y33" s="2"/>
-    </row>
-    <row r="46" spans="15:25" x14ac:dyDescent="0.2">
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="U46" s="2"/>
-      <c r="W46" s="2"/>
-      <c r="Y46" s="2"/>
-    </row>
-    <row r="47" spans="15:25" x14ac:dyDescent="0.2">
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="U47" s="2"/>
-      <c r="W47" s="2"/>
-      <c r="Y47" s="2"/>
-    </row>
-    <row r="56" spans="15:25" x14ac:dyDescent="0.2">
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-      <c r="U56" s="2"/>
-      <c r="W56" s="2"/>
-      <c r="Y56" s="2"/>
-    </row>
-    <row r="57" spans="15:25" x14ac:dyDescent="0.2">
-      <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
-      <c r="U57" s="2"/>
-      <c r="W57" s="2"/>
-      <c r="Y57" s="2"/>
-    </row>
-    <row r="65" spans="15:25" x14ac:dyDescent="0.2">
-      <c r="O65" s="2"/>
-      <c r="P65" s="2"/>
-      <c r="U65" s="2"/>
-      <c r="W65" s="2"/>
-      <c r="Y65" s="2"/>
-    </row>
-    <row r="66" spans="15:25" x14ac:dyDescent="0.2">
-      <c r="O66" s="2"/>
-      <c r="P66" s="2"/>
-      <c r="U66" s="2"/>
-      <c r="W66" s="2"/>
-      <c r="Y66" s="2"/>
+      <c r="X19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" t="s">
+        <v>92</v>
+      </c>
+      <c r="V20" s="2">
+        <v>1</v>
+      </c>
+      <c r="X20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>101</v>
+      </c>
+      <c r="V21" s="2">
+        <v>1</v>
+      </c>
+      <c r="X21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="V22" s="2">
+        <v>1</v>
+      </c>
+      <c r="X22" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" t="s">
+        <v>63</v>
+      </c>
+      <c r="V23" s="2">
+        <v>1</v>
+      </c>
+      <c r="X23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" t="s">
+        <v>102</v>
+      </c>
+      <c r="V24" s="2">
+        <v>1</v>
+      </c>
+      <c r="X24" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" t="s">
+        <v>118</v>
+      </c>
+      <c r="X26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>123</v>
+      </c>
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" t="s">
+        <v>121</v>
+      </c>
+      <c r="X27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="V28" s="2">
+        <v>1</v>
+      </c>
+      <c r="X28" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="V29" s="2">
+        <v>1</v>
+      </c>
+      <c r="X29" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="V30" s="2">
+        <v>1</v>
+      </c>
+      <c r="X30" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="V31" s="2">
+        <v>1</v>
+      </c>
+      <c r="X31" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="V32" s="2">
+        <v>1</v>
+      </c>
+      <c r="X32" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V33" s="2">
+        <v>1</v>
+      </c>
+      <c r="X33" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V34" s="2">
+        <v>1</v>
+      </c>
+      <c r="X34" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V35" s="2">
+        <v>1</v>
+      </c>
+      <c r="X35" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V36" s="2">
+        <v>1</v>
+      </c>
+      <c r="X36" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V37" s="2">
+        <v>1</v>
+      </c>
+      <c r="X37" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+      <c r="V38" s="2">
+        <v>1</v>
+      </c>
+      <c r="X38" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+      <c r="V39" s="2">
+        <v>1</v>
+      </c>
+      <c r="X39" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V40" s="2">
+        <v>1</v>
+      </c>
+      <c r="X40" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V41" s="2">
+        <v>1</v>
+      </c>
+      <c r="X41" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V42" s="2">
+        <v>1</v>
+      </c>
+      <c r="X42" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V43" s="2">
+        <v>1</v>
+      </c>
+      <c r="X43" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V44" s="2">
+        <v>1</v>
+      </c>
+      <c r="X44" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V45" s="2">
+        <v>1</v>
+      </c>
+      <c r="X45" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V46" s="2">
+        <v>1</v>
+      </c>
+      <c r="X46" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V47" s="2">
+        <v>1</v>
+      </c>
+      <c r="X47" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V48" s="2">
+        <v>1</v>
+      </c>
+      <c r="X48" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z48" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V49" s="2">
+        <v>1</v>
+      </c>
+      <c r="X49" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V50" s="2">
+        <v>1</v>
+      </c>
+      <c r="X50" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V51" s="2">
+        <v>1</v>
+      </c>
+      <c r="X51" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="V52" s="2">
+        <v>1</v>
+      </c>
+      <c r="X52" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="P53" s="2"/>
+      <c r="Q53" s="2"/>
+      <c r="V53" s="2">
+        <v>1</v>
+      </c>
+      <c r="X53" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V54" s="2">
+        <v>1</v>
+      </c>
+      <c r="X54" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V55" s="2">
+        <v>1</v>
+      </c>
+      <c r="X55" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V56" s="2">
+        <v>1</v>
+      </c>
+      <c r="X56" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V57" s="2">
+        <v>1</v>
+      </c>
+      <c r="X57" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V58" s="2">
+        <v>1</v>
+      </c>
+      <c r="X58" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V59" s="2">
+        <v>1</v>
+      </c>
+      <c r="X59" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V60" s="2">
+        <v>1</v>
+      </c>
+      <c r="X60" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V61" s="2">
+        <v>1</v>
+      </c>
+      <c r="X61" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="V62" s="2">
+        <v>1</v>
+      </c>
+      <c r="X62" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="P63" s="2"/>
+      <c r="Q63" s="2"/>
+      <c r="V63" s="2">
+        <v>1</v>
+      </c>
+      <c r="X63" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V64" s="2">
+        <v>1</v>
+      </c>
+      <c r="X64" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V65" s="2">
+        <v>1</v>
+      </c>
+      <c r="X65" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V66" s="2">
+        <v>1</v>
+      </c>
+      <c r="X66" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V67" s="2">
+        <v>1</v>
+      </c>
+      <c r="X67" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V68" s="2">
+        <v>1</v>
+      </c>
+      <c r="X68" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V69" s="2">
+        <v>1</v>
+      </c>
+      <c r="X69" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="V70" s="2">
+        <v>1</v>
+      </c>
+      <c r="X70" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="V71" s="2">
+        <v>1</v>
+      </c>
+      <c r="X71" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="16:26" x14ac:dyDescent="0.2">
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2"/>
+      <c r="V72" s="2">
+        <v>1</v>
+      </c>
+      <c r="X72" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z72" s="2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D736743-F982-B748-AF4D-941EEF6BA5FF}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EF3DF2-641B-5E44-AA75-D6FFD80FBD8B}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1297,53 +2076,24 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80EF3DF2-641B-5E44-AA75-D6FFD80FBD8B}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A3DFF1B-7CD7-4048-80C1-413696B477E2}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1352,44 +2102,24 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A3DFF1B-7CD7-4048-80C1-413696B477E2}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6973617B-9497-3C46-9D94-B50EE8137DF9}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="G11" sqref="F11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6973617B-9497-3C46-9D94-B50EE8137DF9}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1398,173 +2128,146 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2753C685-A2C8-074B-AF8C-3877391569BA}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0437A48-3006-3A4F-8E27-223B720E6D4E}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:XFD64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="87" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0437A48-3006-3A4F-8E27-223B720E6D4E}">
-  <dimension ref="A1:B27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="1"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="1"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96314D6-0AFA-A54D-B376-32A53AE93902}">
   <dimension ref="A1:V58"/>
   <sheetViews>
@@ -1595,35 +2298,35 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="P4"/>
       <c r="Q4"/>
       <c r="S4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="T4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="U4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="V4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -1644,13 +2347,13 @@
         <v>models.ForeignKey(Customer,on_delete=models.CASCADE)</v>
       </c>
       <c r="K5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="M5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="N5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="P5"/>
       <c r="Q5"/>
@@ -1689,7 +2392,7 @@
         <v>models.ForeignKey(TaskType,on_delete=models.SET_NULL,null=True)</v>
       </c>
       <c r="K6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="P6"/>
       <c r="Q6"/>
@@ -1728,7 +2431,7 @@
         <v>models.DateTimeField()</v>
       </c>
       <c r="K7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="P7"/>
       <c r="Q7"/>
@@ -1767,7 +2470,7 @@
         <v>models.TextField()</v>
       </c>
       <c r="K8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="P8"/>
       <c r="Q8"/>
@@ -1806,13 +2509,13 @@
         <v>models.ForeignKey(User,on_delete=models.SET_NULL,null=True,related_name='assigned_tasks')</v>
       </c>
       <c r="K9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="O9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="P9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="Q9"/>
       <c r="S9">
@@ -1850,7 +2553,7 @@
         <v>models.CharField(max_length=200)</v>
       </c>
       <c r="K10" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="S10">
         <f t="shared" si="3"/>
@@ -1887,7 +2590,7 @@
         <v>models.CharField(max_length=100)</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="S11">
         <f t="shared" si="3"/>
@@ -1924,7 +2627,7 @@
         <v>models.CharField(max_length=100)</v>
       </c>
       <c r="K12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="S12">
         <f t="shared" si="3"/>
@@ -1961,7 +2664,7 @@
         <v>models.ForeignKey(Employer,on_delete=models.CASCADE)</v>
       </c>
       <c r="K13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="S13">
         <f>FIND("=",K13)</f>
@@ -1998,7 +2701,7 @@
         <v>models.ForeignKey(Organization,on_delete=models.CASCADE)</v>
       </c>
       <c r="K14" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="S14">
         <f t="shared" ref="S14:S24" si="11">FIND("=",K14)</f>
@@ -2035,7 +2738,7 @@
         <v>models.ForeignKey(Organization,on_delete=models.CASCADE)</v>
       </c>
       <c r="K15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="S15">
         <f t="shared" si="11"/>
@@ -2064,7 +2767,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D16" t="e">
         <f t="shared" si="10"/>
@@ -2097,7 +2800,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D17" t="e">
         <f t="shared" si="10"/>
@@ -2130,7 +2833,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D18" t="e">
         <f t="shared" si="10"/>
@@ -2163,7 +2866,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D19" t="e">
         <f t="shared" si="10"/>
@@ -2196,7 +2899,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D20" t="e">
         <f t="shared" si="10"/>
@@ -2229,7 +2932,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D21" t="e">
         <f t="shared" si="10"/>
@@ -2262,7 +2965,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D22" t="e">
         <f t="shared" si="10"/>
@@ -2323,189 +3026,215 @@
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E34" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F34" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="G34" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H34" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="I34" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E37" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G37" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H37" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E40" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E41" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E42" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E43" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E46" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G47" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H47" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="I47" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="J47" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E48" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E51" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G51" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H51" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E54" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E55" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E56" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E57" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E58" t="s">
-        <v>95</v>
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21CEC97-FCED-B744-B683-79B04E4945C6}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2514,22 +3243,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C21CEC97-FCED-B744-B683-79B04E4945C6}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC848DF8-2DCC-D442-88F0-8D70EA2B49CF}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="122.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2537,27 +3275,31 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC848DF8-2DCC-D442-88F0-8D70EA2B49CF}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5DCB6D-D252-554A-AA6D-EF7613AF9735}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="122.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
     </row>
   </sheetData>
@@ -2566,27 +3308,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5DCB6D-D252-554A-AA6D-EF7613AF9735}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCCD04C-73D9-ED48-83F8-2B0724B93DB6}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2594,19 +3334,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCCD04C-73D9-ED48-83F8-2B0724B93DB6}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DE9946-B381-0247-B0AA-E67A7DD58800}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2615,19 +3360,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DE9946-B381-0247-B0AA-E67A7DD58800}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D736743-F982-B748-AF4D-941EEF6BA5FF}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost done with teh excel files and the fake data
</commit_message>
<xml_diff>
--- a/CRUDCreateCode/data/input/models/CRM.xlsx
+++ b/CRUDCreateCode/data/input/models/CRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkax/dev/aimonetize/Backend/DjangoBasic/CRUDCreateCode/data/input/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70DCC33-3605-3340-8B5A-5524CA2453CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA33432-13AF-1446-91AF-1D545E6322DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="760" windowWidth="26180" windowHeight="18880" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
+    <workbookView xWindow="4060" yWindow="760" windowWidth="32340" windowHeight="18880" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="15" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="133">
   <si>
     <t>Variable</t>
   </si>
@@ -406,27 +406,18 @@
     <t>HistoricalRecords()</t>
   </si>
   <si>
-    <t>"History"</t>
-  </si>
-  <si>
     <t>created_at</t>
   </si>
   <si>
     <t>models.DateTimeField(auto_now_add=True)</t>
   </si>
   <si>
-    <t>"created_at"</t>
-  </si>
-  <si>
     <t>updated_at</t>
   </si>
   <si>
     <t>models.DateTimeField(auto_now=True)</t>
   </si>
   <si>
-    <t>"updated_at"</t>
-  </si>
-  <si>
     <t>app_name</t>
   </si>
   <si>
@@ -437,6 +428,39 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>faker_function</t>
+  </si>
+  <si>
+    <t>faker_type</t>
+  </si>
+  <si>
+    <t>Dynamic_User()</t>
+  </si>
+  <si>
+    <t>Dynamic_InteractionType()</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>name()</t>
+  </si>
+  <si>
+    <t>InteractionTimeProvider()</t>
+  </si>
+  <si>
+    <t>Dynamic_Interaction()</t>
+  </si>
+  <si>
+    <t>InteractionDetailsHandledByProvider()</t>
+  </si>
+  <si>
+    <t>Dynamic_TaskType()</t>
+  </si>
+  <si>
+    <t>TaskDueDateProvider()</t>
   </si>
 </sst>
 </file>
@@ -799,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FEED97D-C3FC-F94F-8D67-5465F059E3CB}">
-  <dimension ref="A1:Z72"/>
+  <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,14 +835,14 @@
     <col min="3" max="3" width="13.1640625" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
     <col min="5" max="5" width="88" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
-    <col min="8" max="13" width="11.1640625" customWidth="1"/>
+    <col min="6" max="8" width="32.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" customWidth="1"/>
+    <col min="10" max="15" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -836,69 +860,75 @@
         <v>25</v>
       </c>
       <c r="G1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>24</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>8</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -912,24 +942,30 @@
       <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="V2" s="2">
-        <v>1</v>
-      </c>
-      <c r="W2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="2"/>
       <c r="X2" s="2">
         <v>1</v>
       </c>
+      <c r="Y2" s="2"/>
       <c r="Z2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -938,22 +974,28 @@
         <v>91</v>
       </c>
       <c r="E3" t="s">
-        <v>123</v>
-      </c>
-      <c r="R3" s="2"/>
-      <c r="V3" s="2">
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="F3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" t="s">
+        <v>126</v>
+      </c>
+      <c r="T3" s="2"/>
       <c r="X3" s="2">
         <v>1</v>
       </c>
       <c r="Z3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
         <v>59</v>
@@ -967,21 +1009,27 @@
       <c r="E4" t="s">
         <v>60</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="V4" s="2">
-        <v>1</v>
-      </c>
+      <c r="F4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
       <c r="X4" s="2">
         <v>1</v>
       </c>
       <c r="Z4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
         <v>61</v>
@@ -995,8 +1043,11 @@
       <c r="E5" t="s">
         <v>93</v>
       </c>
-      <c r="V5" s="2">
-        <v>1</v>
+      <c r="F5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" t="s">
+        <v>126</v>
       </c>
       <c r="X5" s="2">
         <v>1</v>
@@ -1004,10 +1055,13 @@
       <c r="Z5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>62</v>
@@ -1021,8 +1075,8 @@
       <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="V6" s="2">
-        <v>1</v>
+      <c r="G6" t="s">
+        <v>6</v>
       </c>
       <c r="X6" s="2">
         <v>1</v>
@@ -1030,10 +1084,13 @@
       <c r="Z6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
         <v>111</v>
@@ -1047,16 +1104,16 @@
       <c r="E7" t="s">
         <v>113</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" t="s">
-        <v>115</v>
       </c>
       <c r="C8" t="s">
         <v>92</v>
@@ -1065,21 +1122,21 @@
         <v>91</v>
       </c>
       <c r="E8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
         <v>116</v>
-      </c>
-      <c r="F8" t="s">
-        <v>117</v>
-      </c>
-      <c r="X8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" t="s">
-        <v>118</v>
       </c>
       <c r="C9" t="s">
         <v>92</v>
@@ -1088,18 +1145,18 @@
         <v>91</v>
       </c>
       <c r="E9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F9" t="s">
-        <v>120</v>
-      </c>
-      <c r="X9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="G9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
         <v>65</v>
@@ -1113,20 +1170,26 @@
       <c r="E10" t="s">
         <v>96</v>
       </c>
-      <c r="O10" s="2"/>
-      <c r="V10" s="2">
-        <v>1</v>
-      </c>
+      <c r="F10" t="s">
+        <v>129</v>
+      </c>
+      <c r="G10" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q10" s="2"/>
       <c r="X10" s="2">
         <v>1</v>
       </c>
       <c r="Z10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
         <v>66</v>
@@ -1140,21 +1203,24 @@
       <c r="E11" t="s">
         <v>63</v>
       </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="V11" s="2">
-        <v>1</v>
-      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
       <c r="X11" s="2">
         <v>1</v>
       </c>
       <c r="Z11" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
         <v>69</v>
@@ -1168,21 +1234,27 @@
       <c r="E12" t="s">
         <v>97</v>
       </c>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="V12" s="2">
-        <v>1</v>
-      </c>
+      <c r="F12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" t="s">
+        <v>126</v>
+      </c>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
       <c r="X12" s="2">
         <v>1</v>
       </c>
       <c r="Z12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B13" t="s">
         <v>111</v>
@@ -1196,16 +1268,16 @@
       <c r="E13" t="s">
         <v>113</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>122</v>
-      </c>
-      <c r="B14" t="s">
-        <v>115</v>
       </c>
       <c r="C14" t="s">
         <v>92</v>
@@ -1214,21 +1286,21 @@
         <v>95</v>
       </c>
       <c r="E14" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" t="s">
         <v>116</v>
-      </c>
-      <c r="F14" t="s">
-        <v>117</v>
-      </c>
-      <c r="X14" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" t="s">
-        <v>118</v>
       </c>
       <c r="C15" t="s">
         <v>92</v>
@@ -1237,18 +1309,18 @@
         <v>95</v>
       </c>
       <c r="E15" t="s">
-        <v>119</v>
-      </c>
-      <c r="F15" t="s">
-        <v>120</v>
-      </c>
-      <c r="X15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -1262,20 +1334,26 @@
       <c r="E16" t="s">
         <v>45</v>
       </c>
-      <c r="S16" s="2"/>
-      <c r="V16" s="2">
-        <v>1</v>
-      </c>
+      <c r="F16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G16" t="s">
+        <v>126</v>
+      </c>
+      <c r="U16" s="2"/>
       <c r="X16" s="2">
         <v>1</v>
       </c>
       <c r="Z16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B17" t="s">
         <v>111</v>
@@ -1289,16 +1367,16 @@
       <c r="E17" t="s">
         <v>113</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" t="s">
-        <v>115</v>
       </c>
       <c r="C18" t="s">
         <v>92</v>
@@ -1307,21 +1385,21 @@
         <v>98</v>
       </c>
       <c r="E18" t="s">
+        <v>115</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" t="s">
         <v>116</v>
-      </c>
-      <c r="F18" t="s">
-        <v>117</v>
-      </c>
-      <c r="X18" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B19" t="s">
-        <v>118</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
@@ -1330,18 +1408,18 @@
         <v>98</v>
       </c>
       <c r="E19" t="s">
-        <v>119</v>
-      </c>
-      <c r="F19" t="s">
-        <v>120</v>
-      </c>
-      <c r="X19" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B20" t="s">
         <v>58</v>
@@ -1353,10 +1431,13 @@
         <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
-      </c>
-      <c r="V20" s="2">
-        <v>1</v>
+        <v>120</v>
+      </c>
+      <c r="F20" t="s">
+        <v>124</v>
+      </c>
+      <c r="G20" t="s">
+        <v>126</v>
       </c>
       <c r="X20" s="2">
         <v>1</v>
@@ -1364,10 +1445,13 @@
       <c r="Z20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B21" t="s">
         <v>72</v>
@@ -1381,8 +1465,11 @@
       <c r="E21" t="s">
         <v>100</v>
       </c>
-      <c r="V21" s="2">
-        <v>1</v>
+      <c r="F21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" t="s">
+        <v>126</v>
       </c>
       <c r="X21" s="2">
         <v>1</v>
@@ -1390,10 +1477,13 @@
       <c r="Z21" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B22" t="s">
         <v>73</v>
@@ -1407,20 +1497,26 @@
       <c r="E22" t="s">
         <v>60</v>
       </c>
-      <c r="T22" s="2"/>
-      <c r="V22" s="2">
-        <v>1</v>
-      </c>
+      <c r="F22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" t="s">
+        <v>59</v>
+      </c>
+      <c r="V22" s="2"/>
       <c r="X22" s="2">
         <v>1</v>
       </c>
       <c r="Z22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB22" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
         <v>74</v>
@@ -1434,8 +1530,8 @@
       <c r="E23" t="s">
         <v>63</v>
       </c>
-      <c r="V23" s="2">
-        <v>1</v>
+      <c r="G23" t="s">
+        <v>6</v>
       </c>
       <c r="X23" s="2">
         <v>1</v>
@@ -1443,10 +1539,13 @@
       <c r="Z23" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B24" t="s">
         <v>75</v>
@@ -1460,8 +1559,11 @@
       <c r="E24" t="s">
         <v>101</v>
       </c>
-      <c r="V24" s="2">
-        <v>1</v>
+      <c r="F24" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" t="s">
+        <v>126</v>
       </c>
       <c r="X24" s="2">
         <v>1</v>
@@ -1469,10 +1571,13 @@
       <c r="Z24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AB24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B25" t="s">
         <v>111</v>
@@ -1486,16 +1591,16 @@
       <c r="E25" t="s">
         <v>113</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B26" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>122</v>
-      </c>
-      <c r="B26" t="s">
-        <v>115</v>
       </c>
       <c r="C26" t="s">
         <v>92</v>
@@ -1504,21 +1609,21 @@
         <v>99</v>
       </c>
       <c r="E26" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B27" t="s">
         <v>116</v>
-      </c>
-      <c r="F26" t="s">
-        <v>117</v>
-      </c>
-      <c r="X26" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" t="s">
-        <v>118</v>
       </c>
       <c r="C27" t="s">
         <v>92</v>
@@ -1527,523 +1632,523 @@
         <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>119</v>
-      </c>
-      <c r="F27" t="s">
-        <v>120</v>
-      </c>
-      <c r="X27" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="V28" s="2">
-        <v>1</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="X28" s="2">
         <v>1</v>
       </c>
       <c r="Z28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="V29" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="X29" s="2">
         <v>1</v>
       </c>
       <c r="Z29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="V30" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="X30" s="2">
         <v>1</v>
       </c>
       <c r="Z30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="V31" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="X31" s="2">
         <v>1</v>
       </c>
       <c r="Z31" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="V32" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="X32" s="2">
         <v>1</v>
       </c>
       <c r="Z32" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V33" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X33" s="2">
         <v>1</v>
       </c>
       <c r="Z33" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V34" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB33" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X34" s="2">
         <v>1</v>
       </c>
       <c r="Z34" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V35" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB34" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X35" s="2">
         <v>1</v>
       </c>
       <c r="Z35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V36" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB35" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X36" s="2">
         <v>1</v>
       </c>
       <c r="Z36" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V37" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X37" s="2">
         <v>1</v>
       </c>
       <c r="Z37" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2"/>
-      <c r="V38" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB37" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="18:28" x14ac:dyDescent="0.2">
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
       <c r="X38" s="2">
         <v>1</v>
       </c>
       <c r="Z38" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2"/>
-      <c r="V39" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="18:28" x14ac:dyDescent="0.2">
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
       <c r="X39" s="2">
         <v>1</v>
       </c>
       <c r="Z39" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V40" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB39" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X40" s="2">
         <v>1</v>
       </c>
       <c r="Z40" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V41" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X41" s="2">
         <v>1</v>
       </c>
       <c r="Z41" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V42" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB41" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X42" s="2">
         <v>1</v>
       </c>
       <c r="Z42" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V43" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB42" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X43" s="2">
         <v>1</v>
       </c>
       <c r="Z43" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V44" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB43" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X44" s="2">
         <v>1</v>
       </c>
       <c r="Z44" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V45" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB44" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X45" s="2">
         <v>1</v>
       </c>
       <c r="Z45" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V46" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB45" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X46" s="2">
         <v>1</v>
       </c>
       <c r="Z46" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V47" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB46" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X47" s="2">
         <v>1</v>
       </c>
       <c r="Z47" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V48" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB47" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X48" s="2">
         <v>1</v>
       </c>
       <c r="Z48" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V49" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB48" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X49" s="2">
         <v>1</v>
       </c>
       <c r="Z49" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V50" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB49" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X50" s="2">
         <v>1</v>
       </c>
       <c r="Z50" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V51" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X51" s="2">
         <v>1</v>
       </c>
       <c r="Z51" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="V52" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="18:28" x14ac:dyDescent="0.2">
+      <c r="R52" s="2"/>
+      <c r="S52" s="2"/>
       <c r="X52" s="2">
         <v>1</v>
       </c>
       <c r="Z52" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-      <c r="V53" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB52" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="18:28" x14ac:dyDescent="0.2">
+      <c r="R53" s="2"/>
+      <c r="S53" s="2"/>
       <c r="X53" s="2">
         <v>1</v>
       </c>
       <c r="Z53" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V54" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB53" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X54" s="2">
         <v>1</v>
       </c>
       <c r="Z54" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V55" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB54" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X55" s="2">
         <v>1</v>
       </c>
       <c r="Z55" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V56" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X56" s="2">
         <v>1</v>
       </c>
       <c r="Z56" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V57" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB56" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X57" s="2">
         <v>1</v>
       </c>
       <c r="Z57" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V58" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB57" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X58" s="2">
         <v>1</v>
       </c>
       <c r="Z58" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V59" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X59" s="2">
         <v>1</v>
       </c>
       <c r="Z59" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V60" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB59" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X60" s="2">
         <v>1</v>
       </c>
       <c r="Z60" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V61" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB60" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X61" s="2">
         <v>1</v>
       </c>
       <c r="Z61" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="P62" s="2"/>
-      <c r="Q62" s="2"/>
-      <c r="V62" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB61" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="18:28" x14ac:dyDescent="0.2">
+      <c r="R62" s="2"/>
+      <c r="S62" s="2"/>
       <c r="X62" s="2">
         <v>1</v>
       </c>
       <c r="Z62" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="P63" s="2"/>
-      <c r="Q63" s="2"/>
-      <c r="V63" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="18:28" x14ac:dyDescent="0.2">
+      <c r="R63" s="2"/>
+      <c r="S63" s="2"/>
       <c r="X63" s="2">
         <v>1</v>
       </c>
       <c r="Z63" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V64" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB63" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X64" s="2">
         <v>1</v>
       </c>
       <c r="Z64" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V65" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB64" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X65" s="2">
         <v>1</v>
       </c>
       <c r="Z65" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V66" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB65" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X66" s="2">
         <v>1</v>
       </c>
       <c r="Z66" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V67" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB66" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X67" s="2">
         <v>1</v>
       </c>
       <c r="Z67" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V68" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB67" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X68" s="2">
         <v>1</v>
       </c>
       <c r="Z68" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V69" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB68" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X69" s="2">
         <v>1</v>
       </c>
       <c r="Z69" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="V70" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB69" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="18:28" x14ac:dyDescent="0.2">
       <c r="X70" s="2">
         <v>1</v>
       </c>
       <c r="Z70" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="P71" s="2"/>
-      <c r="Q71" s="2"/>
-      <c r="V71" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="18:28" x14ac:dyDescent="0.2">
+      <c r="R71" s="2"/>
+      <c r="S71" s="2"/>
       <c r="X71" s="2">
         <v>1</v>
       </c>
       <c r="Z71" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="16:26" x14ac:dyDescent="0.2">
-      <c r="P72" s="2"/>
-      <c r="Q72" s="2"/>
-      <c r="V72" s="2">
-        <v>1</v>
-      </c>
+      <c r="AB71" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="18:28" x14ac:dyDescent="0.2">
+      <c r="R72" s="2"/>
+      <c r="S72" s="2"/>
       <c r="X72" s="2">
         <v>1</v>
       </c>
       <c r="Z72" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB72" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2064,7 +2169,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -2090,7 +2195,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -2116,7 +2221,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -2146,7 +2251,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -2157,7 +2262,7 @@
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>91</v>
@@ -2168,7 +2273,7 @@
     </row>
     <row r="3" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
         <v>91</v>
@@ -2179,7 +2284,7 @@
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
         <v>95</v>
@@ -2190,7 +2295,7 @@
     </row>
     <row r="5" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
         <v>95</v>
@@ -2201,7 +2306,7 @@
     </row>
     <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
         <v>98</v>
@@ -2212,7 +2317,7 @@
     </row>
     <row r="7" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
         <v>98</v>
@@ -2223,7 +2328,7 @@
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B8" t="s">
         <v>99</v>
@@ -2234,7 +2339,7 @@
     </row>
     <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
         <v>99</v>
@@ -2245,7 +2350,7 @@
     </row>
     <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
         <v>90</v>
@@ -2256,7 +2361,7 @@
     </row>
     <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B11" t="s">
         <v>90</v>
@@ -3231,7 +3336,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -3260,7 +3365,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -3293,7 +3398,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -3322,7 +3427,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -3348,7 +3453,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>
@@ -3374,7 +3479,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
added automation for django and flask app producer, consumer and more
</commit_message>
<xml_diff>
--- a/CRUDCreateCode/data/input/models/CRM.xlsx
+++ b/CRUDCreateCode/data/input/models/CRM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tkax/dev/aimonetize/Backend/DjangoBasic/CRUDCreateCode/data/input/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA33432-13AF-1446-91AF-1D545E6322DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46AA6B8-7EC2-1C4F-B0B0-FB97F639C270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4060" yWindow="760" windowWidth="32340" windowHeight="18880" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
+    <workbookView xWindow="4020" yWindow="740" windowWidth="32340" windowHeight="18880" xr2:uid="{43DD2820-FE61-F645-B31F-194723807C3A}"/>
   </bookViews>
   <sheets>
     <sheet name="model" sheetId="15" r:id="rId1"/>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FEED97D-C3FC-F94F-8D67-5465F059E3CB}">
   <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>